<commit_message>
building work study excel
</commit_message>
<xml_diff>
--- a/clocking.xlsx
+++ b/clocking.xlsx
@@ -14,29 +14,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
-  <si>
-    <t>cvcvcvcvcvcvcvcv</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>hahaha</t>
-  </si>
-  <si>
-    <t>2017/01/19 14:59</t>
-  </si>
-  <si>
-    <t>2017/01/19 15:00</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+  <si>
+    <t>everton mendozaholmes</t>
+  </si>
+  <si>
+    <t>Gary Tsai</t>
+  </si>
+  <si>
+    <t>0FD8AD9C60</t>
+  </si>
+  <si>
+    <t>CFD893A460</t>
   </si>
   <si>
     <t>2017/01/19 15:03</t>
   </si>
   <si>
+    <t>2017/01/19 18:59</t>
+  </si>
+  <si>
+    <t>2017/01/19 19:00</t>
+  </si>
+  <si>
     <t>2017/01/19 15:04</t>
   </si>
   <si>
@@ -119,20 +119,58 @@
   </si>
   <si>
     <t>2017/01/19 16:04</t>
+  </si>
+  <si>
+    <t>2017/01/19 17:28</t>
+  </si>
+  <si>
+    <t>2017/01/19 17:35</t>
+  </si>
+  <si>
+    <t>2017/01/19 17:44</t>
+  </si>
+  <si>
+    <t>2017/01/19 17:46</t>
+  </si>
+  <si>
+    <t>2017/01/19 18:00</t>
+  </si>
+  <si>
+    <t>2017/01/19 18:09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt formatCode="General" numFmtId="164"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,14 +190,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="5" name="Percent" xfId="3"/>
+    <cellStyle builtinId="4" name="Currency" xfId="4"/>
+    <cellStyle builtinId="3" name="Comma" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -451,323 +505,376 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A129" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F145" activeCellId="0" pane="topLeft" sqref="F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="15.1020408163265"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row customHeight="1" ht="15" r="1" s="2" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row customHeight="1" ht="15" r="2" s="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row customHeight="1" ht="15" r="3" s="2" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="4" s="2" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+    <row customHeight="1" ht="15" r="5" s="2" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+    <row customHeight="1" ht="15" r="6" s="2" spans="1:2">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+    <row customHeight="1" ht="15" r="7" s="2" spans="1:2">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+    <row customHeight="1" ht="15" r="8" s="2" spans="1:2">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
+    <row customHeight="1" ht="15" r="9" s="2" spans="1:2">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
+    <row customHeight="1" ht="15" r="10" s="2" spans="1:2">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
+    <row customHeight="1" ht="15" r="11" s="2" spans="1:2">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
+    <row customHeight="1" ht="15" r="12" s="2" spans="1:2">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
+    <row customHeight="1" ht="15" r="13" s="2" spans="1:2">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
+    <row customHeight="1" ht="15" r="14" s="2" spans="1:2">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
+    <row customHeight="1" ht="15" r="15" s="2" spans="1:2">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
+    <row customHeight="1" ht="15" r="16" s="2" spans="1:2">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
+    <row customHeight="1" ht="15" r="17" s="2" spans="1:2">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
+    <row customHeight="1" ht="15" r="18" s="2" spans="1:2">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
+    <row customHeight="1" ht="15" r="19" s="2" spans="1:2">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
+    <row customHeight="1" ht="15" r="20" s="2" spans="1:2">
+      <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
+    <row customHeight="1" ht="15" r="21" s="2" spans="1:2">
+      <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
+    <row customHeight="1" ht="15" r="22" s="2" spans="1:2">
+      <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
+    <row customHeight="1" ht="15" r="23" s="2" spans="1:2">
+      <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
+    <row customHeight="1" ht="15" r="24" s="2" spans="1:2">
+      <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
+    <row customHeight="1" ht="15" r="25" s="2" spans="1:2">
+      <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
+    <row customHeight="1" ht="15" r="26" s="2" spans="1:2">
+      <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
+    <row customHeight="1" ht="15" r="27" s="2" spans="1:2">
+      <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
+    <row customHeight="1" ht="15" r="28" s="2" spans="1:2">
+      <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
+    <row customHeight="1" ht="15" r="29" s="2" spans="1:2">
+      <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
+    <row customHeight="1" ht="15" r="30" s="2" spans="1:2">
+      <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
+    <row customHeight="1" ht="15" r="31" s="2" spans="1:2">
+      <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
+    <row customHeight="1" ht="15" r="32" s="2" spans="1:2">
+      <c r="A32" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
+    <row customHeight="1" ht="15" r="33" s="2" spans="1:2">
+      <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
+    <row customHeight="1" ht="15" r="34" s="2" spans="1:2">
+      <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
+    <row customHeight="1" ht="15" r="35" s="2" spans="1:2">
+      <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
+    <row customHeight="1" ht="15" r="36" s="2" spans="1:2">
+      <c r="A36" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
+    <row customHeight="1" ht="15" r="37" s="2" spans="1:2">
+      <c r="A37" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
+    <row customHeight="1" ht="15" r="38" s="2" spans="1:2">
+      <c r="A38" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
+    <row customHeight="1" ht="15" r="39" s="2" spans="1:2">
+      <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="s">
+    <row customHeight="1" ht="15" r="40" s="2" spans="1:2">
+      <c r="A40" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
+    <row customHeight="1" ht="15" r="41" s="2" spans="1:2">
+      <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
+    <row customHeight="1" ht="15" r="42" s="2" spans="1:2">
+      <c r="A42" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
+    <row customHeight="1" ht="15" r="43" s="2" spans="1:2">
+      <c r="A43" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
+    <row customHeight="1" ht="15" r="44" s="2" spans="1:2">
+      <c r="A44" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
+    <row customHeight="1" ht="15" r="45" s="2" spans="1:2">
+      <c r="A45" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
+    <row customHeight="1" ht="15" r="46" s="2" spans="1:2">
+      <c r="A46" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
+    <row customHeight="1" ht="15" r="47" s="2" spans="1:2">
+      <c r="A47" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
+    <row customHeight="1" ht="15" r="48" s="2" spans="1:2">
+      <c r="A48" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" t="s">
+    <row customHeight="1" ht="15" r="49" s="2" spans="1:2">
+      <c r="A49" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" t="s">
+    <row customHeight="1" ht="15" r="50" s="2" spans="1:2">
+      <c r="A50" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
+    <row customHeight="1" ht="15" r="51" s="2" spans="1:2">
+      <c r="A51" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
+    <row customHeight="1" ht="15" r="52" s="2" spans="1:2">
+      <c r="A52" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
+    <row customHeight="1" ht="15" r="53" s="2" spans="1:2">
+      <c r="A53" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
+    <row customHeight="1" ht="15" r="54" s="2" spans="1:2">
+      <c r="A54" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
+    <row customHeight="1" ht="15" r="55" s="2" spans="1:2">
+      <c r="A55" s="1" t="s">
         <v>34</v>
       </c>
     </row>
+    <row customHeight="1" ht="15" r="56" s="2" spans="1:2">
+      <c r="A56" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="57" s="2" spans="1:2">
+      <c r="A57" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="58" s="2" spans="1:2">
+      <c r="A58" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="59" s="2" spans="1:2">
+      <c r="A59" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="60" s="2" spans="1:2">
+      <c r="A60" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="61" s="2" spans="1:2">
+      <c r="A61" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="62" s="2" spans="1:2">
+      <c r="A62" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="63" s="2" spans="1:2">
+      <c r="A63" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="64" s="2" spans="1:2">
+      <c r="A64" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="65" s="2" spans="1:2">
+      <c r="A65" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="66" s="2" spans="1:2">
+      <c r="A66" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="67" s="2" spans="1:2">
+      <c r="A67" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="68" s="2" spans="1:2">
+      <c r="A68" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
enhanced work study log
</commit_message>
<xml_diff>
--- a/clocking.xlsx
+++ b/clocking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>everton mendozaholmes</t>
   </si>
@@ -22,28 +22,64 @@
     <t>Gary Tsai</t>
   </si>
   <si>
+    <t>Anthony Avevor</t>
+  </si>
+  <si>
+    <t>Vanessa Cordero</t>
+  </si>
+  <si>
     <t>0FD8AD9C60</t>
   </si>
   <si>
     <t>CFD893A460</t>
   </si>
   <si>
+    <t>8FD8A5E5E0</t>
+  </si>
+  <si>
+    <t>CFD8A948E0</t>
+  </si>
+  <si>
     <t>2017/01/19 15:03</t>
   </si>
   <si>
     <t>2017/01/19 18:59</t>
   </si>
   <si>
+    <t>2017/01/24 14:28</t>
+  </si>
+  <si>
+    <t>2017/01/24 14:48</t>
+  </si>
+  <si>
     <t>2017/01/19 19:00</t>
   </si>
   <si>
+    <t>2017/01/24 14:37</t>
+  </si>
+  <si>
     <t>2017/01/19 15:04</t>
   </si>
   <si>
+    <t>2017/01/24 14:26</t>
+  </si>
+  <si>
+    <t>2017/01/24 14:39</t>
+  </si>
+  <si>
     <t>2017/01/19 15:05</t>
   </si>
   <si>
+    <t>IN -&gt; 2017/01/24 14:56</t>
+  </si>
+  <si>
     <t>2017/01/19 15:06</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/01/24 14:56</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/01/24 14:57</t>
   </si>
   <si>
     <t>2017/01/19 15:15</t>
@@ -191,10 +227,10 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
@@ -208,12 +244,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="5" name="Percent" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="0"/>
+    <cellStyle builtinId="5" name="Percent" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="3"/>
     <cellStyle builtinId="4" name="Currency" xfId="4"/>
-    <cellStyle builtinId="3" name="Comma" xfId="5"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -509,7 +545,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A129" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="F145" activeCellId="0" pane="topLeft" sqref="F145"/>
@@ -517,359 +553,405 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="1" width="15.1020408163265"/>
+    <col customWidth="1" max="1" min="1" style="2" width="25"/>
+    <col customWidth="1" max="1" min="1" style="2" width="25"/>
+    <col customWidth="1" max="2" min="2" style="2" width="25"/>
+    <col customWidth="1" max="2" min="2" style="2" width="25"/>
+    <col customWidth="1" max="3" min="3" style="2" width="25"/>
+    <col customWidth="1" max="3" min="3" style="2" width="25"/>
+    <col customWidth="1" max="4" min="4" style="2" width="25"/>
+    <col customWidth="1" max="4" min="4" style="2" width="25"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="2" spans="1:2">
+    <row customHeight="1" ht="15" r="1" s="2" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="2" s="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="2" s="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="3" s="2" spans="1:2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="3" s="2" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="4" s="2" spans="1:2">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="4" s="2" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="5" s="2" spans="1:2">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="5" s="2" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="6" s="2" spans="1:2">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="6" s="2" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="7" s="2" spans="1:2">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="7" s="2" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="8" s="2" spans="1:2">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="8" s="2" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="9" s="2" spans="1:2">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="9" s="2" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="10" s="2" spans="1:2">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="10" s="2" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="11" s="2" spans="1:2">
+        <v>19</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="11" s="2" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="12" s="2" spans="1:2">
+        <v>19</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="12" s="2" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="13" s="2" spans="1:2">
+        <v>22</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="13" s="2" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="14" s="2" spans="1:2">
+        <v>23</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="14" s="2" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="15" s="2" spans="1:2">
+        <v>24</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="15" s="2" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="16" s="2" spans="1:2">
+        <v>25</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="16" s="2" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="17" s="2" spans="1:2">
+        <v>26</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="17" s="2" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="18" s="2" spans="1:2">
+        <v>26</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="18" s="2" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="19" s="2" spans="1:2">
+        <v>27</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="19" s="2" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="20" s="2" spans="1:2">
+        <v>28</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="20" s="2" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="21" s="2" spans="1:2">
+        <v>28</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="21" s="2" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="22" s="2" spans="1:2">
+        <v>28</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="22" s="2" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="23" s="2" spans="1:2">
+        <v>29</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="23" s="2" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="24" s="2" spans="1:2">
+        <v>30</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="24" s="2" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="25" s="2" spans="1:2">
+        <v>30</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="25" s="2" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="26" s="2" spans="1:2">
+        <v>30</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="26" s="2" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="27" s="2" spans="1:2">
+        <v>30</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="27" s="2" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="28" s="2" spans="1:2">
+        <v>30</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="28" s="2" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="29" s="2" spans="1:2">
+        <v>31</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="29" s="2" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="30" s="2" spans="1:2">
+        <v>31</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="30" s="2" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="31" s="2" spans="1:2">
+        <v>31</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="31" s="2" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="32" s="2" spans="1:2">
+        <v>31</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="32" s="2" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="33" s="2" spans="1:2">
+        <v>32</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="33" s="2" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="34" s="2" spans="1:2">
+        <v>32</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="34" s="2" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="35" s="2" spans="1:2">
+        <v>32</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="35" s="2" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="36" s="2" spans="1:2">
+        <v>33</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="36" s="2" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="37" s="2" spans="1:2">
+        <v>33</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="37" s="2" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="38" s="2" spans="1:2">
+        <v>34</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="38" s="2" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="39" s="2" spans="1:2">
+        <v>35</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="39" s="2" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="40" s="2" spans="1:2">
+        <v>36</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="40" s="2" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="41" s="2" spans="1:2">
+        <v>37</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="41" s="2" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="42" s="2" spans="1:2">
+        <v>38</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="42" s="2" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="43" s="2" spans="1:2">
+        <v>39</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="43" s="2" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="44" s="2" spans="1:2">
+        <v>40</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="44" s="2" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="45" s="2" spans="1:2">
+        <v>41</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="45" s="2" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="46" s="2" spans="1:2">
+        <v>41</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="46" s="2" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="47" s="2" spans="1:2">
+        <v>42</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="47" s="2" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="48" s="2" spans="1:2">
+        <v>42</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="48" s="2" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="49" s="2" spans="1:2">
+        <v>43</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="49" s="2" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="50" s="2" spans="1:2">
+        <v>43</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="50" s="2" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="51" s="2" spans="1:2">
+        <v>43</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="51" s="2" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="52" s="2" spans="1:2">
+        <v>44</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="52" s="2" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="53" s="2" spans="1:2">
+        <v>45</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="53" s="2" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="54" s="2" spans="1:2">
+        <v>45</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="54" s="2" spans="1:4">
       <c r="A54" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="55" s="2" spans="1:2">
+        <v>46</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="55" s="2" spans="1:4">
       <c r="A55" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="56" s="2" spans="1:2">
+        <v>46</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="56" s="2" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="57" s="2" spans="1:2">
+        <v>47</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="57" s="2" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="58" s="2" spans="1:2">
+        <v>48</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="58" s="2" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="59" s="2" spans="1:2">
+        <v>49</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="59" s="2" spans="1:4">
       <c r="A59" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="60" s="2" spans="1:2">
+        <v>49</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="60" s="2" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="61" s="2" spans="1:2">
+        <v>49</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="61" s="2" spans="1:4">
       <c r="A61" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="62" s="2" spans="1:2">
+        <v>50</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="62" s="2" spans="1:4">
       <c r="A62" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="63" s="2" spans="1:2">
+        <v>50</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="63" s="2" spans="1:4">
       <c r="A63" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="64" s="2" spans="1:2">
+        <v>50</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="64" s="2" spans="1:4">
       <c r="A64" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="65" s="2" spans="1:2">
+        <v>51</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="65" s="2" spans="1:4">
       <c r="A65" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="66" s="2" spans="1:2">
+        <v>51</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="66" s="2" spans="1:4">
       <c r="A66" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="67" s="2" spans="1:2">
+        <v>51</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="67" s="2" spans="1:4">
       <c r="A67" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="68" s="2" spans="1:2">
+        <v>52</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="68" s="2" spans="1:4">
       <c r="A68" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified work study feature
</commit_message>
<xml_diff>
--- a/clocking.xlsx
+++ b/clocking.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
+  <sheets>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>everton mendozaholmes</t>
   </si>
@@ -82,10 +82,22 @@
     <t>IN -&gt; 2017/01/24 14:57</t>
   </si>
   <si>
+    <t>OUT -&gt; 2017/01/26 14:52</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/01/26 14:53</t>
+  </si>
+  <si>
     <t>2017/01/19 15:15</t>
   </si>
   <si>
+    <t>OUT -&gt; 2017/01/26 15:28</t>
+  </si>
+  <si>
     <t>2017/01/19 15:16</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/01/26 15:28</t>
   </si>
   <si>
     <t>2017/01/19 15:19</t>
@@ -227,21 +239,21 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="7" name="Currency [0]" xfId="0"/>
@@ -251,7 +263,6 @@
     <cellStyle builtinId="4" name="Currency" xfId="4"/>
     <cellStyle builtinId="6" name="Comma [0]" xfId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -551,15 +562,15 @@
       <selection activeCell="F145" activeCellId="0" pane="topLeft" sqref="F145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="2" width="25"/>
-    <col customWidth="1" max="1" min="1" style="2" width="25"/>
-    <col customWidth="1" max="2" min="2" style="2" width="25"/>
-    <col customWidth="1" max="2" min="2" style="2" width="25"/>
-    <col customWidth="1" max="3" min="3" style="2" width="25"/>
-    <col customWidth="1" max="3" min="3" style="2" width="25"/>
-    <col customWidth="1" max="4" min="4" style="2" width="25"/>
+    <col customWidth="1" max="1" min="1" style="2" width="40"/>
+    <col customWidth="1" max="1" min="1" style="2" width="40"/>
+    <col customWidth="1" max="2" min="2" style="2" width="40"/>
+    <col customWidth="1" max="2" min="2" style="2" width="40"/>
+    <col customWidth="1" max="3" min="3" style="2" width="40"/>
+    <col customWidth="1" max="3" min="3" style="2" width="40"/>
+    <col customWidth="1" max="4" min="4" style="2" width="40"/>
     <col customWidth="1" max="4" min="4" style="2" width="25"/>
   </cols>
   <sheetData>
@@ -663,295 +674,307 @@
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="11" s="2" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="12" s="2" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="13" s="2" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="14" s="2" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="15" s="2" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="16" s="2" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="17" s="2" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="18" s="2" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="19" s="2" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="20" s="2" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="21" s="2" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="22" s="2" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="23" s="2" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="24" s="2" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="25" s="2" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="26" s="2" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="27" s="2" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="28" s="2" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="29" s="2" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="30" s="2" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="31" s="2" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="32" s="2" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="33" s="2" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="34" s="2" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="35" s="2" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="36" s="2" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="37" s="2" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="38" s="2" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="39" s="2" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="40" s="2" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="41" s="2" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="42" s="2" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="43" s="2" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="44" s="2" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="45" s="2" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="46" s="2" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="47" s="2" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="48" s="2" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="49" s="2" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="50" s="2" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="51" s="2" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="52" s="2" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="53" s="2" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="54" s="2" spans="1:4">
       <c r="A54" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="55" s="2" spans="1:4">
       <c r="A55" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="56" s="2" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="57" s="2" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="58" s="2" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="59" s="2" spans="1:4">
       <c r="A59" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="60" s="2" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="61" s="2" spans="1:4">
       <c r="A61" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="62" s="2" spans="1:4">
       <c r="A62" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="63" s="2" spans="1:4">
       <c r="A63" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="64" s="2" spans="1:4">
       <c r="A64" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="65" s="2" spans="1:4">
       <c r="A65" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="66" s="2" spans="1:4">
       <c r="A66" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="67" s="2" spans="1:4">
       <c r="A67" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="68" s="2" spans="1:4">
       <c r="A68" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug in reporting column for reporting
</commit_message>
<xml_diff>
--- a/clocking.xlsx
+++ b/clocking.xlsx
@@ -14,12 +14,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
-  <si>
-    <t>8FD8ADBD20</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+  <si>
+    <t>arango juan</t>
+  </si>
+  <si>
+    <t>Gary Tsai</t>
+  </si>
+  <si>
+    <t>Covalky Pena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystal Evelyn </t>
+  </si>
+  <si>
+    <t>Jean Augustin</t>
+  </si>
+  <si>
+    <t>Natalie Primus</t>
+  </si>
+  <si>
+    <t>Miguel Martillo</t>
+  </si>
+  <si>
+    <t>Anne Crosby</t>
+  </si>
+  <si>
+    <t>CFD8AFA4C0</t>
+  </si>
+  <si>
+    <t>CFD893A460</t>
+  </si>
+  <si>
+    <t>0FD8AD42A0</t>
+  </si>
+  <si>
+    <t>0FD8A87380</t>
+  </si>
+  <si>
+    <t>4FD8B36A40</t>
+  </si>
+  <si>
+    <t>0FD8AE8B60</t>
+  </si>
+  <si>
+    <t>8FD8B68DE0</t>
+  </si>
+  <si>
+    <t>4FD8A33DE0</t>
   </si>
   <si>
     <t>IN -&gt; 2017/01/31 18:57</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/01/31 19:12</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/01/31 19:19</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/01/31 19:23</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/01/31 19:24</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/01 08:49</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/01 09:06</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/01 09:08</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/01/31 19:07</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/01/31 19:12</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/01 15:25</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/01 17:09</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/01 17:52</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/01/31 19:23</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/01/31 19:26</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/01/31 19:33</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/01 15:01</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/01 17:31</t>
   </si>
 </sst>
 </file>
@@ -76,9 +172,9 @@
   <cellStyleXfs count="6">
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
@@ -88,12 +184,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="7" name="Currency [0]" xfId="0"/>
-    <cellStyle builtinId="5" name="Percent" xfId="1"/>
-    <cellStyle builtinId="4" name="Currency" xfId="2"/>
-    <cellStyle builtinId="3" name="Comma" xfId="3"/>
-    <cellStyle builtinId="0" name="Normal" xfId="4"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="0"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="3" name="Comma" xfId="4"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -389,7 +485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:A3"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
@@ -405,16 +501,139 @@
     <col customWidth="1" max="3" min="3" style="1" width="40"/>
     <col customWidth="1" max="4" min="4" style="1" width="40"/>
     <col customWidth="1" max="4" min="4" style="1" width="40"/>
+    <col customWidth="1" max="5" min="5" style="1" width="40"/>
+    <col customWidth="1" max="5" min="5" style="1" width="40"/>
+    <col customWidth="1" max="6" min="6" style="1" width="40"/>
+    <col customWidth="1" max="6" min="6" style="1" width="40"/>
+    <col customWidth="1" max="7" min="7" style="1" width="40"/>
+    <col customWidth="1" max="7" min="7" style="1" width="40"/>
+    <col customWidth="1" max="8" min="8" style="1" width="40"/>
+    <col customWidth="1" max="8" min="8" style="1" width="40"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bugs on reporting.py
</commit_message>
<xml_diff>
--- a/clocking.xlsx
+++ b/clocking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
   <si>
     <t>John Orellana</t>
   </si>
@@ -64,7 +64,124 @@
     <t>OUT -&gt; 2017/02/07 12:21</t>
   </si>
   <si>
+    <t>OUT -&gt; 2017/02/10 07:42</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/14 14:11</t>
+  </si>
+  <si>
     <t>OUT -&gt; 2017/02/08 20:52</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/14 08:23</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/10 18:03</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/16 14:29</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/15 13:02</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/15 13:37</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/14 16:29</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/23 11:46</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/16 16:39</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/16 10:43</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/15 14:03</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/22 20:10</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/16 14:29</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/15 20:50</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/23 17:26</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/28 08:07</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/17 07:53</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/28 14:56</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/01 14:13</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/21 14:04</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/21 16:26</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/21 19:01</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/22 13:42</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/22 20:50</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/22 20:50</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/24 07:57</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/24 17:54</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/24 17:54</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/27 20:30</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/28 14:16</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/28 16:26</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/28 16:27</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/01 14:27</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/01 18:06</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/01 20:47</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/02 16:24</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/02 16:25</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/03 11:13</t>
   </si>
 </sst>
 </file>
@@ -119,12 +236,12 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -133,12 +250,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="5" name="Percent" xfId="1"/>
-    <cellStyle builtinId="3" name="Comma" xfId="2"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="3"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="4"/>
-    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="0"/>
+    <cellStyle builtinId="4" name="Currency" xfId="1"/>
+    <cellStyle builtinId="5" name="Percent" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="3" name="Comma" xfId="4"/>
+    <cellStyle builtinId="0" name="Normal" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -434,7 +551,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B12" activeCellId="0" pane="topLeft" sqref="B12"/>
@@ -518,8 +635,188 @@
       <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="C31" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>